<commit_message>
Updated Hybrid framework with all runmode set to N
</commit_message>
<xml_diff>
--- a/HybridRediff/Files/PortfolioSuite.xlsx
+++ b/HybridRediff/Files/PortfolioSuite.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -567,14 +567,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.5546875" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -590,7 +590,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -598,7 +598,7 @@
         <v>22</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -606,7 +606,7 @@
         <v>25</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -622,14 +622,14 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.85546875" customWidth="1"/>
-    <col min="6" max="6" width="21.28515625" customWidth="1"/>
+    <col min="4" max="4" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.88671875" customWidth="1"/>
+    <col min="6" max="6" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -952,17 +952,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12:C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="29.140625" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" customWidth="1"/>
+    <col min="3" max="3" width="29.109375" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" customWidth="1"/>
+    <col min="5" max="5" width="18.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">

</xml_diff>